<commit_message>
Add folder of docs for used png and bg
</commit_message>
<xml_diff>
--- a/Report/Booking Analysis Report.xlsx
+++ b/Report/Booking Analysis Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prafull Wahatule\Desktop\Booking Analysis\Report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7E5B05-FE92-4F16-836C-55CB2562C100}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88CAD62-4A48-4A62-B440-9C45DF1D5AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="3" xr2:uid="{982E9D42-EB19-4268-B625-6FDCA404ACAD}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="252">
   <si>
     <t>Rows After</t>
   </si>
@@ -323,13 +323,7 @@
     <t xml:space="preserve">mearge 3 coloumn  </t>
   </si>
   <si>
-    <t xml:space="preserve"> (arrival_date) = (arrival_date_year)+(arrival_date_month)+(arrival_date_day_of_month)</t>
-  </si>
-  <si>
     <t>Final</t>
-  </si>
-  <si>
-    <t>column Name</t>
   </si>
   <si>
     <t>booking_id</t>
@@ -923,6 +917,24 @@
   </si>
   <si>
     <t>Ribbon Chart</t>
+  </si>
+  <si>
+    <t>Performed Activity</t>
+  </si>
+  <si>
+    <t>(arrival_date) = (arrival_date_year)+(arrival_date_month)+(arrival_date_day_of_month)</t>
+  </si>
+  <si>
+    <t>Add Primary Key</t>
+  </si>
+  <si>
+    <t>Befor Transformation</t>
+  </si>
+  <si>
+    <t>After Transformation</t>
+  </si>
+  <si>
+    <t>Transformation</t>
   </si>
 </sst>
 </file>
@@ -1193,9 +1205,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -1269,6 +1278,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1586,7 +1596,7 @@
   <dimension ref="B2:P14"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1617,7 +1627,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="14"/>
-      <c r="E3" s="16"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="8" t="s">
         <v>79</v>
       </c>
@@ -1645,7 +1655,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="14"/>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>1</v>
       </c>
       <c r="F4" s="10">
@@ -1675,7 +1685,7 @@
         <v>6</v>
       </c>
       <c r="D5" s="14"/>
-      <c r="E5" s="17">
+      <c r="E5" s="16">
         <v>2</v>
       </c>
       <c r="F5" s="10">
@@ -1705,7 +1715,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="14"/>
-      <c r="E6" s="17">
+      <c r="E6" s="16">
         <v>3</v>
       </c>
       <c r="F6" s="10">
@@ -1735,7 +1745,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="14"/>
-      <c r="E7" s="17">
+      <c r="E7" s="16">
         <v>4</v>
       </c>
       <c r="F7" s="10">
@@ -1765,7 +1775,7 @@
         <v>90</v>
       </c>
       <c r="D8" s="14"/>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>5</v>
       </c>
       <c r="F8" s="10">
@@ -1794,13 +1804,13 @@
         <v>6</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D9" s="14"/>
-      <c r="E9" s="17">
+      <c r="E9" s="16">
         <v>6</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <f>G8</f>
         <v>87220</v>
       </c>
@@ -1825,15 +1835,15 @@
         <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="E10" s="17">
+        <v>97</v>
+      </c>
+      <c r="E10" s="16">
         <v>7</v>
       </c>
       <c r="F10" s="10">
         <v>87220</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="17">
         <v>87220</v>
       </c>
       <c r="H10" s="12">
@@ -1854,19 +1864,19 @@
         <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="17">
+        <v>98</v>
+      </c>
+      <c r="E11" s="16">
         <v>8</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <f>G10</f>
         <v>87220</v>
       </c>
       <c r="G11" s="10">
         <v>87220</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="18">
         <f>F11-G11</f>
         <v>0</v>
       </c>
@@ -1885,19 +1895,19 @@
         <v>9</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E12" s="17">
+        <v>98</v>
+      </c>
+      <c r="E12" s="16">
         <v>9</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <f>G11</f>
         <v>87220</v>
       </c>
       <c r="G12" s="10">
         <v>87220</v>
       </c>
-      <c r="H12" s="19">
+      <c r="H12" s="18">
         <f>F12-G12</f>
         <v>0</v>
       </c>
@@ -1916,19 +1926,19 @@
         <v>10</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="E13" s="17">
+        <v>100</v>
+      </c>
+      <c r="E13" s="16">
         <v>10</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <f>G12</f>
         <v>87220</v>
       </c>
       <c r="G13" s="10">
         <v>86605</v>
       </c>
-      <c r="H13" s="19">
+      <c r="H13" s="18">
         <f>F13-G13</f>
         <v>615</v>
       </c>
@@ -1949,17 +1959,17 @@
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="16">
         <v>11</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <f>G13</f>
         <v>86605</v>
       </c>
       <c r="G14" s="10">
         <v>86605</v>
       </c>
-      <c r="H14" s="20">
+      <c r="H14" s="19">
         <v>0</v>
       </c>
       <c r="I14" s="2">
@@ -1980,10 +1990,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F8B0D9-F8C0-4197-BF3C-EC40092398E1}">
-  <dimension ref="B3:H36"/>
+  <dimension ref="B2:H37"/>
   <sheetViews>
     <sheetView zoomScale="71" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:G31"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1991,558 +2001,594 @@
     <col min="2" max="2" width="15.88671875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="53.5546875" customWidth="1"/>
-    <col min="7" max="7" width="28.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="15.6">
-      <c r="B3" s="4" t="s">
+    <row r="2" spans="2:8" ht="15.6">
+      <c r="C2" s="48" t="s">
+        <v>249</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="15.6">
+      <c r="B4" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="15" t="s">
+      <c r="F4" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="15.6">
-      <c r="B4" s="2">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="15.6">
       <c r="B5" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>93</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="F5" s="54">
+        <v>1</v>
+      </c>
+      <c r="G5" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="2:8" ht="15.6">
       <c r="B6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="54">
+        <v>2</v>
+      </c>
+      <c r="G6" s="54" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="2:8" ht="15.6">
+      <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F6">
+      <c r="F7" s="54">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" s="54" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="2:8" ht="18" customHeight="1">
-      <c r="B7" s="2">
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="2:8" ht="18" customHeight="1">
+      <c r="B8" s="2">
         <v>4</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F7">
+      <c r="F8" s="54">
         <v>4</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" s="54" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" ht="15.6">
-      <c r="B8" s="2">
-        <v>5</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8" t="s">
-        <v>96</v>
-      </c>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="2:8" ht="15.6">
       <c r="B9" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="F9" s="54">
+        <v>5</v>
+      </c>
+      <c r="G9" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="2:8" ht="15.6">
       <c r="B10" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10">
-        <v>7</v>
-      </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F10" s="54">
+        <v>6</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:8" ht="15.6">
       <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="54">
+        <v>7</v>
+      </c>
+      <c r="G11" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.6">
+      <c r="B12" s="2">
         <v>8</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F11">
+      <c r="F12" s="54">
         <v>8</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" s="54" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" ht="31.2">
-      <c r="B12" s="2">
-        <v>9</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12">
-        <v>9</v>
-      </c>
-      <c r="G12" t="s">
-        <v>97</v>
-      </c>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="2:8" ht="31.2">
       <c r="B13" s="2">
+        <v>9</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="54">
+        <v>9</v>
+      </c>
+      <c r="G13" s="54" t="s">
+        <v>95</v>
+      </c>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="2:8" ht="31.2">
+      <c r="B14" s="2">
         <v>10</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F13">
+      <c r="F14" s="54">
         <v>10</v>
       </c>
-      <c r="G13" t="s">
+      <c r="G14" s="54" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" ht="15.6">
-      <c r="B14" s="2">
-        <v>11</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14">
-        <v>11</v>
-      </c>
-      <c r="G14" t="s">
-        <v>87</v>
-      </c>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="2:8" ht="15.6">
       <c r="B15" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
-        <v>23</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="F15" s="54">
+        <v>11</v>
+      </c>
+      <c r="G15" s="54" t="s">
+        <v>87</v>
+      </c>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="2:8" ht="15.6">
       <c r="B16" s="2">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="54">
+        <v>12</v>
+      </c>
+      <c r="G16" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:8" ht="15.6">
+      <c r="B17" s="2">
         <v>13</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="F16">
+      <c r="F17" s="54">
         <v>13</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G17" s="54" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" ht="31.2">
-      <c r="B17" s="2">
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="2:8" ht="31.2">
+      <c r="B18" s="2">
         <v>14</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F17">
+      <c r="F18" s="54">
         <v>14</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G18" s="54" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" ht="15.6">
-      <c r="B18" s="2">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="2:8" ht="15.6">
+      <c r="B19" s="2">
         <v>15</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F18">
+      <c r="F19" s="54">
         <v>15</v>
       </c>
-      <c r="G18" t="s">
+      <c r="G19" s="54" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" ht="31.2">
-      <c r="B19" s="2">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="2:8" ht="31.2">
+      <c r="B20" s="2">
         <v>16</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F19">
+      <c r="F20" s="54">
         <v>16</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" s="54" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" ht="31.2">
-      <c r="B20" s="2">
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="2:8" ht="31.2">
+      <c r="B21" s="2">
         <v>17</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C21" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F20">
+      <c r="F21" s="54">
         <v>17</v>
       </c>
-      <c r="G20" t="s">
+      <c r="G21" s="54" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" ht="15.6">
-      <c r="B21" s="2">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="2:8" ht="15.6">
+      <c r="B22" s="2">
         <v>18</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F21">
+      <c r="F22" s="54">
         <v>18</v>
       </c>
-      <c r="G21" t="s">
+      <c r="G22" s="54" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" ht="15.6">
-      <c r="B22" s="2">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="2:8" ht="15.6">
+      <c r="B23" s="2">
         <v>19</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="F22">
+      <c r="F23" s="54">
         <v>19</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" s="54" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" ht="31.2">
-      <c r="B23" s="2">
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="2:8" ht="31.2">
+      <c r="B24" s="2">
         <v>20</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F23">
+      <c r="F24" s="54">
         <v>20</v>
       </c>
-      <c r="G23" t="s">
+      <c r="G24" s="54" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" ht="15.6">
-      <c r="B24" s="2">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="2:8" ht="15.6">
+      <c r="B25" s="2">
         <v>21</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F24">
+      <c r="F25" s="54">
         <v>21</v>
       </c>
-      <c r="G24" t="s">
+      <c r="G25" s="54" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" ht="15.6">
-      <c r="B25" s="2">
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="2:8" ht="15.6">
+      <c r="B26" s="2">
         <v>22</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F25">
+      <c r="F26" s="54">
         <v>22</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G26" s="54" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" ht="15.6">
-      <c r="B26" s="2">
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="2:8" ht="15.6">
+      <c r="B27" s="2">
         <v>23</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="C27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F26">
+      <c r="F27" s="54">
         <v>23</v>
       </c>
-      <c r="G26" t="s">
+      <c r="G27" s="54" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="2:7" ht="31.2">
-      <c r="B27" s="2">
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="2:8" ht="31.2">
+      <c r="B28" s="2">
         <v>24</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C28" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F27">
+      <c r="F28" s="54">
         <v>24</v>
       </c>
-      <c r="G27" t="s">
+      <c r="G28" s="54" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" ht="31.2">
-      <c r="B28" s="2">
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="2:8" ht="31.2">
+      <c r="B29" s="2">
         <v>25</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F28">
+      <c r="F29" s="54">
         <v>25</v>
       </c>
-      <c r="G28" t="s">
+      <c r="G29" s="54" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="29" spans="2:7" ht="31.2">
-      <c r="B29" s="2">
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="2:8" ht="31.2">
+      <c r="B30" s="2">
         <v>26</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C30" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F29">
+      <c r="F30" s="54">
         <v>26</v>
       </c>
-      <c r="G29" t="s">
+      <c r="G30" s="54" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="30" spans="2:7" ht="15.6">
-      <c r="B30" s="2">
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="2:8" ht="15.6">
+      <c r="B31" s="2">
         <v>27</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F30">
+      <c r="F31" s="54">
         <v>27</v>
       </c>
-      <c r="G30" t="s">
+      <c r="G31" s="54" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="31" spans="2:7" ht="31.2">
-      <c r="B31" s="2">
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="2:8" ht="31.2">
+      <c r="B32" s="2">
         <v>28</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F31">
+      <c r="F32" s="54">
         <v>28</v>
       </c>
-      <c r="G31" t="s">
+      <c r="G32" s="54" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="2:7" ht="15.6">
-      <c r="B32" s="2">
-        <v>29</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:4" ht="15.6">
       <c r="B33" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="15.6">
       <c r="B34" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="15.6">
       <c r="B35" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="15.6">
       <c r="B36" s="2">
+        <v>32</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15.6">
+      <c r="B37" s="2">
         <v>33</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C37" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -2553,134 +2599,153 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{780C279F-2B82-4095-9029-39A0509AF4C9}">
-  <dimension ref="B3:D13"/>
+  <dimension ref="B2:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="85.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
-      <c r="B3">
+    <row r="2" spans="2:4" ht="15.6">
+      <c r="C2" s="48" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" ht="15.6">
+      <c r="B4" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="15.6">
+      <c r="B5" s="54">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="2:4">
-      <c r="B4">
+      <c r="D5" s="6" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="15.6">
+      <c r="B6" s="54">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C6" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4">
-      <c r="B5">
+      <c r="D6" s="6" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="15.6">
+      <c r="B7" s="54">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
-      <c r="B6">
+    <row r="8" spans="2:4" ht="15.6">
+      <c r="B8" s="54">
         <v>4</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C8" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D8" s="6" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
-      <c r="B7">
+    <row r="9" spans="2:4" ht="15.6">
+      <c r="B9" s="54">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D9" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
-      <c r="B8">
+    <row r="10" spans="2:4" ht="15.6">
+      <c r="B10" s="54">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" s="6" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
-      <c r="B9">
+    <row r="11" spans="2:4" ht="15.6">
+      <c r="B11" s="54">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D9" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4">
-      <c r="B10">
+      <c r="D11" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="15.6">
+      <c r="B12" s="54">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4">
-      <c r="B11">
+      <c r="D12" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="15.6">
+      <c r="B13" s="54">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
-      <c r="B12">
+    <row r="14" spans="2:4" ht="15.6">
+      <c r="B14" s="54">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D14" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
-      <c r="B13">
+    <row r="15" spans="2:4" ht="15.6">
+      <c r="B15" s="54">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" t="s">
-        <v>110</v>
+      <c r="C15" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -2690,10 +2755,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC310175-FF74-49CD-BEDC-3226069E4333}">
-  <dimension ref="B2:W40"/>
+  <dimension ref="B4:W42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2715,874 +2780,874 @@
     <col min="22" max="22" width="34.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" ht="20.399999999999999">
-      <c r="B2" s="29" t="s">
-        <v>187</v>
-      </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="I2" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="P2" s="31" t="s">
+    <row r="4" spans="2:21" ht="20.399999999999999">
+      <c r="B4" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="I4" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="P4" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" ht="15.6">
+      <c r="D6" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="F6" s="40" t="s">
+        <v>78</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="J6" s="48" t="s">
+        <v>5</v>
+      </c>
+      <c r="K6" s="48" t="s">
+        <v>116</v>
+      </c>
+      <c r="L6" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="M6" s="48" t="s">
+        <v>124</v>
+      </c>
+      <c r="N6" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q6" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="R6" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="S6" s="37" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="15.6">
-      <c r="D4" s="41" t="s">
+    <row r="7" spans="2:21" ht="18">
+      <c r="D7" s="41">
+        <v>1</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="L7" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>1</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="S7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="U7" s="21"/>
+    </row>
+    <row r="8" spans="2:21" ht="18">
+      <c r="D8" s="41">
+        <v>2</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="G8" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="J8" s="6">
+        <v>2</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="L8" s="38" t="s">
+        <v>123</v>
+      </c>
+      <c r="M8" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>2</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="U8" s="21"/>
+    </row>
+    <row r="9" spans="2:21" ht="18">
+      <c r="D9" s="41">
+        <v>3</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="G9" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" s="6">
+        <v>3</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="L9" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>3</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="U9" s="21"/>
+    </row>
+    <row r="10" spans="2:21" ht="18">
+      <c r="D10" s="41">
+        <v>4</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="J10" s="6">
+        <v>4</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="L10" s="38" t="s">
+        <v>137</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="U10" s="21"/>
+    </row>
+    <row r="11" spans="2:21" ht="18">
+      <c r="D11" s="41">
         <v>5</v>
       </c>
-      <c r="E4" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="F4" s="41" t="s">
+      <c r="E11" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="G11" s="43" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="15.6">
+      <c r="D12" s="41">
+        <v>6</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="G12" s="43" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="2:21">
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="2:21">
+      <c r="G14" s="22"/>
+    </row>
+    <row r="15" spans="2:21" ht="20.399999999999999">
+      <c r="B15" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="20"/>
+      <c r="D15" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="I15" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="P15" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="2:21">
+      <c r="G16" s="22"/>
+    </row>
+    <row r="17" spans="2:23" ht="15.6">
+      <c r="D17" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="40" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4" s="49" t="s">
+      <c r="G17" s="40" t="s">
+        <v>106</v>
+      </c>
+      <c r="J17" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="L4" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="M4" s="49" t="s">
-        <v>126</v>
-      </c>
-      <c r="N4" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q4" s="38" t="s">
+      <c r="K17" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="L17" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="M17" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="N17" s="36" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q17" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="R4" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="S4" s="38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" ht="18">
-      <c r="D5" s="42">
-        <v>1</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="G5" s="44" t="s">
-        <v>114</v>
-      </c>
-      <c r="J5" s="6">
-        <v>1</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="L5" s="48" t="s">
-        <v>124</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="Q5" s="6">
-        <v>1</v>
-      </c>
-      <c r="R5" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="S5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="U5" s="22"/>
-    </row>
-    <row r="6" spans="2:21" ht="18">
-      <c r="D6" s="42">
-        <v>2</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="G6" s="44" t="s">
-        <v>115</v>
-      </c>
-      <c r="J6" s="6">
-        <v>2</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="L6" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q6" s="6">
-        <v>2</v>
-      </c>
-      <c r="R6" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="S6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="U6" s="22"/>
-    </row>
-    <row r="7" spans="2:21" ht="18">
-      <c r="D7" s="42">
-        <v>3</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="G7" s="44" t="s">
-        <v>116</v>
-      </c>
-      <c r="J7" s="6">
-        <v>3</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="L7" s="48" t="s">
-        <v>10</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="Q7" s="6">
-        <v>3</v>
-      </c>
-      <c r="R7" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="S7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="U7" s="22"/>
-    </row>
-    <row r="8" spans="2:21" ht="18">
-      <c r="D8" s="42">
-        <v>4</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>105</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="G8" s="44" t="s">
-        <v>117</v>
-      </c>
-      <c r="J8" s="6">
-        <v>4</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="L8" s="39" t="s">
-        <v>139</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>130</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="U8" s="22"/>
-    </row>
-    <row r="9" spans="2:21" ht="18">
-      <c r="D9" s="42">
-        <v>5</v>
-      </c>
-      <c r="E9" s="43" t="s">
-        <v>106</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="G9" s="44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="2:21" ht="15.6">
-      <c r="D10" s="42">
-        <v>6</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>112</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="G10" s="44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="2:21">
-      <c r="F11" s="24"/>
-    </row>
-    <row r="12" spans="2:21">
-      <c r="G12" s="23"/>
-    </row>
-    <row r="13" spans="2:21" ht="20.399999999999999">
-      <c r="B13" s="29" t="s">
-        <v>188</v>
-      </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="G13" s="23"/>
-      <c r="I13" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="P13" s="31" t="s">
+      <c r="R17" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="S17" s="37" t="s">
         <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="2:21">
-      <c r="G14" s="23"/>
-    </row>
-    <row r="15" spans="2:21" ht="15.6">
-      <c r="D15" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" s="40" t="s">
-        <v>78</v>
-      </c>
-      <c r="G15" s="41" t="s">
-        <v>108</v>
-      </c>
-      <c r="J15" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="K15" s="50" t="s">
-        <v>118</v>
-      </c>
-      <c r="L15" s="50" t="s">
-        <v>123</v>
-      </c>
-      <c r="M15" s="50" t="s">
-        <v>126</v>
-      </c>
-      <c r="N15" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q15" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="R15" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="S15" s="38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="16" spans="2:21" ht="18">
-      <c r="D16" s="6">
-        <v>1</v>
-      </c>
-      <c r="E16" s="47" t="s">
-        <v>140</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="G16" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="J16" s="6">
-        <v>1</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="M16" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q16" s="6">
-        <v>1</v>
-      </c>
-      <c r="R16" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="S16" s="39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="2:23" ht="18">
-      <c r="D17" s="6">
-        <v>2</v>
-      </c>
-      <c r="E17" s="47" t="s">
-        <v>141</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="G17" s="46" t="s">
-        <v>153</v>
-      </c>
-      <c r="J17" s="6">
-        <v>2</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="M17" s="48" t="s">
-        <v>145</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q17" s="6">
-        <v>2</v>
-      </c>
-      <c r="R17" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="S17" s="39" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="18" spans="2:23" ht="18">
       <c r="D18" s="6">
-        <v>3</v>
-      </c>
-      <c r="E18" s="47" t="s">
-        <v>142</v>
+        <v>1</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>138</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="G18" s="45" t="s">
-        <v>154</v>
+        <v>217</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>153</v>
       </c>
       <c r="J18" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K18" s="6" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="L18" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="M18" s="48" t="s">
-        <v>127</v>
+        <v>156</v>
+      </c>
+      <c r="M18" s="47" t="s">
+        <v>129</v>
       </c>
       <c r="N18" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="R18" s="25"/>
-      <c r="S18" s="25"/>
+        <v>225</v>
+      </c>
+      <c r="Q18" s="6">
+        <v>1</v>
+      </c>
+      <c r="R18" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="S18" s="38" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="19" spans="2:23" ht="18">
       <c r="D19" s="6">
+        <v>2</v>
+      </c>
+      <c r="E19" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="G19" s="45" t="s">
+        <v>151</v>
+      </c>
+      <c r="J19" s="6">
+        <v>2</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="M19" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>2</v>
+      </c>
+      <c r="R19" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="S19" s="38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" ht="18">
+      <c r="D20" s="6">
+        <v>3</v>
+      </c>
+      <c r="E20" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>152</v>
+      </c>
+      <c r="J20" s="6">
+        <v>3</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="M20" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
+    </row>
+    <row r="21" spans="2:23" ht="18">
+      <c r="D21" s="6">
         <v>4</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E21" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>154</v>
+      </c>
+      <c r="J21" s="6">
+        <v>4</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="M21" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" ht="18">
+      <c r="G22" s="22"/>
+      <c r="J22" s="6">
+        <v>5</v>
+      </c>
+      <c r="K22" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="M22" s="47" t="s">
         <v>149</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="G19" s="45" t="s">
-        <v>156</v>
-      </c>
-      <c r="J19" s="6">
-        <v>4</v>
-      </c>
-      <c r="K19" s="6" t="s">
+      <c r="N22" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23">
+      <c r="G23" s="22"/>
+    </row>
+    <row r="24" spans="2:23">
+      <c r="G24" s="22"/>
+    </row>
+    <row r="25" spans="2:23" ht="20.399999999999999">
+      <c r="B25" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="D25" s="27" t="s">
         <v>161</v>
       </c>
-      <c r="L19" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="M19" s="48" t="s">
-        <v>146</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="20" spans="2:23" ht="18">
-      <c r="G20" s="23"/>
-      <c r="J20" s="6">
+      <c r="I25" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="P25" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" ht="18">
+      <c r="D27" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="K20" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="L20" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="M20" s="48" t="s">
-        <v>151</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="21" spans="2:23">
-      <c r="G21" s="23"/>
-    </row>
-    <row r="22" spans="2:23">
-      <c r="G22" s="23"/>
-    </row>
-    <row r="23" spans="2:23" ht="20.399999999999999">
-      <c r="B23" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>163</v>
-      </c>
-      <c r="I23" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="P23" s="31" t="s">
+      <c r="E27" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="J27" s="50" t="s">
+        <v>5</v>
+      </c>
+      <c r="K27" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="L27" s="50" t="s">
+        <v>121</v>
+      </c>
+      <c r="M27" s="50" t="s">
+        <v>181</v>
+      </c>
+      <c r="N27" s="50" t="s">
+        <v>182</v>
+      </c>
+      <c r="O27" s="25"/>
+      <c r="Q27" s="37" t="s">
+        <v>5</v>
+      </c>
+      <c r="R27" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="S27" s="37" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="25" spans="2:23" ht="18">
-      <c r="D25" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="36" t="s">
-        <v>107</v>
-      </c>
-      <c r="F25" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G25" s="36" t="s">
-        <v>108</v>
-      </c>
-      <c r="J25" s="51" t="s">
-        <v>5</v>
-      </c>
-      <c r="K25" s="51" t="s">
-        <v>118</v>
-      </c>
-      <c r="L25" s="51" t="s">
-        <v>123</v>
-      </c>
-      <c r="M25" s="51" t="s">
-        <v>183</v>
-      </c>
-      <c r="N25" s="51" t="s">
-        <v>184</v>
-      </c>
-      <c r="O25" s="26"/>
-      <c r="Q25" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="R25" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="S25" s="38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="26" spans="2:23" ht="18">
-      <c r="D26" s="6">
-        <v>1</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="G26" s="6"/>
-      <c r="J26" s="52">
-        <v>1</v>
-      </c>
-      <c r="K26" s="52" t="s">
-        <v>232</v>
-      </c>
-      <c r="L26" s="52" t="s">
-        <v>233</v>
-      </c>
-      <c r="M26" s="52" t="s">
-        <v>129</v>
-      </c>
-      <c r="N26" s="52" t="s">
-        <v>241</v>
-      </c>
-      <c r="O26" s="27"/>
-      <c r="Q26" s="6">
-        <v>3</v>
-      </c>
-      <c r="R26" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="S26" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="W26" s="22"/>
-    </row>
-    <row r="27" spans="2:23" ht="18">
-      <c r="D27" s="6">
-        <v>2</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="G27" s="6"/>
-      <c r="J27" s="52">
-        <v>2</v>
-      </c>
-      <c r="K27" s="52" t="s">
-        <v>234</v>
-      </c>
-      <c r="L27" s="52" t="s">
-        <v>235</v>
-      </c>
-      <c r="M27" s="52" t="s">
-        <v>236</v>
-      </c>
-      <c r="N27" s="52" t="s">
-        <v>242</v>
-      </c>
-      <c r="O27" s="27"/>
-      <c r="Q27" s="6">
-        <v>4</v>
-      </c>
-      <c r="R27" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="S27" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="W27" s="22"/>
     </row>
     <row r="28" spans="2:23" ht="18">
       <c r="D28" s="6">
+        <v>1</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G28" s="6"/>
+      <c r="J28" s="51">
+        <v>1</v>
+      </c>
+      <c r="K28" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="L28" s="51" t="s">
+        <v>231</v>
+      </c>
+      <c r="M28" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="N28" s="51" t="s">
+        <v>239</v>
+      </c>
+      <c r="O28" s="26"/>
+      <c r="Q28" s="6">
         <v>3</v>
       </c>
-      <c r="E28" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="G28" s="6"/>
-      <c r="J28" s="52">
-        <v>3</v>
-      </c>
-      <c r="K28" s="52" t="s">
-        <v>237</v>
-      </c>
-      <c r="L28" s="52" t="s">
-        <v>238</v>
-      </c>
-      <c r="M28" s="52" t="s">
-        <v>236</v>
-      </c>
-      <c r="N28" s="52" t="s">
-        <v>243</v>
-      </c>
-      <c r="O28" s="27"/>
-      <c r="W28" s="22"/>
+      <c r="R28" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="S28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="W28" s="21"/>
     </row>
     <row r="29" spans="2:23" ht="18">
       <c r="D29" s="6">
+        <v>2</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="G29" s="6"/>
+      <c r="J29" s="51">
+        <v>2</v>
+      </c>
+      <c r="K29" s="51" t="s">
+        <v>232</v>
+      </c>
+      <c r="L29" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="M29" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="N29" s="51" t="s">
+        <v>240</v>
+      </c>
+      <c r="O29" s="26"/>
+      <c r="Q29" s="6">
         <v>4</v>
       </c>
-      <c r="E29" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="G29" s="6"/>
-      <c r="J29" s="52">
-        <v>4</v>
-      </c>
-      <c r="K29" s="52" t="s">
-        <v>170</v>
-      </c>
-      <c r="L29" s="52" t="s">
+      <c r="R29" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="M29" s="52" t="s">
-        <v>168</v>
-      </c>
-      <c r="N29" s="52" t="s">
-        <v>244</v>
-      </c>
-      <c r="O29" s="27"/>
-      <c r="W29" s="22"/>
+      <c r="S29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="W29" s="21"/>
     </row>
     <row r="30" spans="2:23" ht="18">
       <c r="D30" s="6">
+        <v>3</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G30" s="6"/>
+      <c r="J30" s="51">
+        <v>3</v>
+      </c>
+      <c r="K30" s="51" t="s">
+        <v>235</v>
+      </c>
+      <c r="L30" s="51" t="s">
+        <v>236</v>
+      </c>
+      <c r="M30" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="N30" s="51" t="s">
+        <v>241</v>
+      </c>
+      <c r="O30" s="26"/>
+      <c r="W30" s="21"/>
+    </row>
+    <row r="31" spans="2:23" ht="18">
+      <c r="D31" s="6">
+        <v>4</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="G31" s="6"/>
+      <c r="J31" s="51">
+        <v>4</v>
+      </c>
+      <c r="K31" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="L31" s="51" t="s">
+        <v>167</v>
+      </c>
+      <c r="M31" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="N31" s="51" t="s">
+        <v>242</v>
+      </c>
+      <c r="O31" s="26"/>
+      <c r="W31" s="21"/>
+    </row>
+    <row r="32" spans="2:23" ht="18">
+      <c r="D32" s="6">
         <v>5</v>
       </c>
-      <c r="E30" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="F30" s="6" t="s">
+      <c r="E32" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="G32" s="6"/>
+      <c r="J32" s="51">
+        <v>5</v>
+      </c>
+      <c r="K32" s="51" t="s">
+        <v>183</v>
+      </c>
+      <c r="L32" s="51" t="s">
+        <v>184</v>
+      </c>
+      <c r="M32" s="51" t="s">
+        <v>165</v>
+      </c>
+      <c r="N32" s="51" t="s">
+        <v>243</v>
+      </c>
+      <c r="O32" s="26"/>
+    </row>
+    <row r="33" spans="2:19" ht="18">
+      <c r="J33" s="51">
+        <v>6</v>
+      </c>
+      <c r="K33" s="51" t="s">
+        <v>237</v>
+      </c>
+      <c r="L33" s="51" t="s">
+        <v>238</v>
+      </c>
+      <c r="M33" s="52" t="s">
+        <v>245</v>
+      </c>
+      <c r="N33" s="51" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19">
+      <c r="M34" s="26"/>
+    </row>
+    <row r="36" spans="2:19" ht="21.6">
+      <c r="B36" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="C36" s="20"/>
+      <c r="D36" s="31" t="s">
+        <v>161</v>
+      </c>
+      <c r="I36" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="P36" s="30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" ht="15.6">
+      <c r="D38" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>189</v>
+      </c>
+      <c r="F38" s="34" t="s">
+        <v>190</v>
+      </c>
+      <c r="G38" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="N38" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="G30" s="6"/>
-      <c r="J30" s="52">
+      <c r="Q38" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="K30" s="52" t="s">
-        <v>185</v>
-      </c>
-      <c r="L30" s="52" t="s">
-        <v>186</v>
-      </c>
-      <c r="M30" s="52" t="s">
-        <v>167</v>
-      </c>
-      <c r="N30" s="52" t="s">
-        <v>245</v>
-      </c>
-      <c r="O30" s="27"/>
-    </row>
-    <row r="31" spans="2:23" ht="18">
-      <c r="J31" s="52">
-        <v>6</v>
-      </c>
-      <c r="K31" s="52" t="s">
-        <v>239</v>
-      </c>
-      <c r="L31" s="52" t="s">
-        <v>240</v>
-      </c>
-      <c r="M31" s="53" t="s">
-        <v>247</v>
-      </c>
-      <c r="N31" s="52" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="32" spans="2:23">
-      <c r="M32" s="27"/>
-    </row>
-    <row r="34" spans="2:19" ht="21.6">
-      <c r="B34" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="C34" s="21"/>
-      <c r="D34" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="I34" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="P34" s="31" t="s">
+      <c r="R38" s="37" t="s">
+        <v>131</v>
+      </c>
+      <c r="S38" s="37" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="36" spans="2:19" ht="15.6">
-      <c r="D36" s="35" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="35" t="s">
+    <row r="39" spans="2:19" ht="15.6">
+      <c r="D39" s="2">
+        <v>1</v>
+      </c>
+      <c r="E39" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F36" s="35" t="s">
+      <c r="F39" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="G36" s="35" t="s">
-        <v>108</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="N36" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="Q36" s="38" t="s">
-        <v>5</v>
-      </c>
-      <c r="R36" s="38" t="s">
-        <v>133</v>
-      </c>
-      <c r="S36" s="38" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="37" spans="2:19" ht="15.6">
-      <c r="D37" s="2">
+      <c r="G39" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="J39" s="2">
         <v>1</v>
       </c>
-      <c r="E37" s="2" t="s">
+      <c r="K39" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="L39" s="32" t="s">
+        <v>207</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q39" s="6">
+        <v>2</v>
+      </c>
+      <c r="R39" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="S39" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" ht="15.6">
+      <c r="D40" s="2">
+        <v>2</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F40" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="G40" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="J40" s="2">
+        <v>2</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="L40" s="32" t="s">
+        <v>208</v>
+      </c>
+      <c r="M40" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q40" s="6">
+        <v>3</v>
+      </c>
+      <c r="R40" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="S40" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" ht="31.2">
+      <c r="D41" s="2">
+        <v>3</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G37" s="54" t="s">
+      <c r="F41" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G41" s="53" t="s">
         <v>198</v>
       </c>
-      <c r="J37" s="2">
-        <v>1</v>
-      </c>
-      <c r="K37" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="L37" s="33" t="s">
+      <c r="J41" s="2">
+        <v>3</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L41" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="M37" s="2" t="s">
+      <c r="M41" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q41" s="6">
+        <v>4</v>
+      </c>
+      <c r="R41" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="S41" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" ht="15.6">
+      <c r="J42" s="2">
+        <v>4</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="L42" s="32" t="s">
+        <v>210</v>
+      </c>
+      <c r="M42" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="N37" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="Q37" s="6">
-        <v>2</v>
-      </c>
-      <c r="R37" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="S37" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="38" spans="2:19" ht="15.6">
-      <c r="D38" s="2">
-        <v>2</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="G38" s="54" t="s">
-        <v>199</v>
-      </c>
-      <c r="J38" s="2">
-        <v>2</v>
-      </c>
-      <c r="K38" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="L38" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q38" s="6">
-        <v>3</v>
-      </c>
-      <c r="R38" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="S38" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="2:19" ht="31.2">
-      <c r="D39" s="2">
-        <v>3</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G39" s="54" t="s">
-        <v>200</v>
-      </c>
-      <c r="J39" s="2">
-        <v>3</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="L39" s="33" t="s">
-        <v>211</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="N39" s="2" t="s">
+      <c r="N42" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="Q39" s="6">
-        <v>4</v>
-      </c>
-      <c r="R39" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="S39" s="6" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="2:19" ht="15.6">
-      <c r="J40" s="2">
-        <v>4</v>
-      </c>
-      <c r="K40" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="L40" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="N40" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>